<commit_message>
change details about git usage guide document
</commit_message>
<xml_diff>
--- a/Git Project Management Tool/git.xlsx
+++ b/Git Project Management Tool/git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jansson\Desktop\Full-stack\Git Project Management Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099067C8-CB68-4157-A27F-5DD0346136B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F83471-B8E9-408B-BDB1-521839822C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26070" yWindow="2565" windowWidth="20055" windowHeight="10575" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="导航栏" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="176">
   <si>
     <t>1. cd命令：改变目录</t>
   </si>
@@ -565,18 +565,6 @@
     <t>2. 克隆项目代码</t>
   </si>
   <si>
-    <t>创建Pull Request（在GitHub/GitLab等平台上）</t>
-  </si>
-  <si>
-    <t>同事审查代码，提供反馈</t>
-  </si>
-  <si>
-    <t>根据反馈修改代码，继续推送更新</t>
-  </si>
-  <si>
-    <t>获得批准后，合并到主分支（通常是通过平台的UI操作）</t>
-  </si>
-  <si>
     <t>处理冲突</t>
   </si>
   <si>
@@ -679,18 +667,6 @@
     <t>日常开发流程：git pull 获取最新的远程更改</t>
   </si>
   <si>
-    <t>3创建新分支进行开发：git checkout -b feature/new-feature</t>
-  </si>
-  <si>
-    <t>4编写代码，进行本地提交：git add . 和 git commit -m "描述"</t>
-  </si>
-  <si>
-    <t>5定期推送分支到远程：git push origin feature/new-feature</t>
-  </si>
-  <si>
-    <t>6 代码审查和合并</t>
-  </si>
-  <si>
     <t>老师</t>
   </si>
   <si>
@@ -728,6 +704,36 @@
   </si>
   <si>
     <t>99 100</t>
+  </si>
+  <si>
+    <t>3. 创建新分支进行开发：git checkout -b &lt;feature/new-feature&gt;</t>
+  </si>
+  <si>
+    <t>&lt;feature/new-feature&gt;本地文件名</t>
+  </si>
+  <si>
+    <t>建议在合并到main之前：</t>
+  </si>
+  <si>
+    <t>4. 编写代码，进行本地提交：git add . 和 git commit -m "描述"</t>
+  </si>
+  <si>
+    <t>5. 把main的最新代码合并到你的功能分支：git merge main</t>
+  </si>
+  <si>
+    <t>5. 把功能开发代码合并到main分支：git push origin main</t>
+  </si>
+  <si>
+    <t>6. 主分支定期推送到远程分仓库</t>
+  </si>
+  <si>
+    <t>7. 代码审查和合并</t>
+  </si>
+  <si>
+    <t>同事审查代码，提供反馈； 根据反馈修改代码，继续推送更新</t>
+  </si>
+  <si>
+    <t>获得批准后，合并到主分支</t>
   </si>
 </sst>
 </file>
@@ -2544,6 +2550,390 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0AFCCC8-D6FF-FED0-CB73-8189C0D2004C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3390899" y="14049376"/>
+          <a:ext cx="3781425" cy="904874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git checkout main  # </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>切换到</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>main</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>分支</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git pull origin main # </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>拉取</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>main</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>分支最新代码</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git checkout your-feature-branch  # </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>切回你的功能分支</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git merge main  # </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>把</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>main</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>的最新代码合并到你的分支</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D989597-EB91-4F3B-9C33-E8085379510D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3333750" y="15563851"/>
+          <a:ext cx="4714875" cy="495299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git checkout main #</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>确认功能没问题后，切换到</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>main</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>分支合并功能分支</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git merge feature/your-branch</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A49E7D-FC6C-4C64-9C81-528F95E6FEF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3343276" y="16554450"/>
+          <a:ext cx="2533650" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git push origin feature/your-branch</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03AD8DB6-3B46-4CDA-B4CE-85B5D9ACE6CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3038475" y="18211800"/>
+          <a:ext cx="4714875" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git checkout main</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git pull</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git merge feature/your-branch</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>git push origin main</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3388,7 +3778,7 @@
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3489,13 +3879,13 @@
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" s="4" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="18:27" x14ac:dyDescent="0.25">
       <c r="R68" s="1"/>
       <c r="S68" s="13" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -3504,15 +3894,15 @@
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
       <c r="Z68" s="13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="AA68" s="4" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="18:27" x14ac:dyDescent="0.25">
       <c r="R69" s="15" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="S69" s="15"/>
       <c r="T69" s="15"/>
@@ -3522,10 +3912,10 @@
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
       <c r="Z69" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA69" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="AA69" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="70" spans="18:27" x14ac:dyDescent="0.25">
@@ -3535,12 +3925,12 @@
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
       <c r="W70" s="13" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
       <c r="Z70" s="13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="18:27" x14ac:dyDescent="0.25">
@@ -3564,7 +3954,7 @@
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
       <c r="Z72" s="13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="18:27" x14ac:dyDescent="0.25">
@@ -3579,10 +3969,10 @@
       <c r="X73" s="1"/>
       <c r="Y73" s="1"/>
       <c r="Z73" s="14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="AA73" s="4" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3992,10 +4382,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC8E6EB-D299-468C-92E1-93201DF9EC15}">
-  <dimension ref="E2:W87"/>
+  <dimension ref="E2:W109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="L106" sqref="L106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5228,82 +5618,113 @@
     </row>
     <row r="61" spans="5:23" x14ac:dyDescent="0.25">
       <c r="F61" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="5:23" x14ac:dyDescent="0.25">
       <c r="F63" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E81" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E91" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E76" s="1" t="s">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="1" t="s">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E80" s="1" t="s">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="1" t="s">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="1" t="s">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="1" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -5324,7 +5745,7 @@
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -5334,7 +5755,7 @@
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5344,7 +5765,7 @@
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -5354,7 +5775,7 @@
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -5364,7 +5785,7 @@
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -5374,7 +5795,7 @@
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -5384,7 +5805,7 @@
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -5394,7 +5815,7 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -5404,7 +5825,7 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -5414,7 +5835,7 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -5424,7 +5845,7 @@
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -5434,7 +5855,7 @@
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -5444,7 +5865,7 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5454,7 +5875,7 @@
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -5464,7 +5885,7 @@
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -5474,7 +5895,7 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -5484,7 +5905,7 @@
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5494,7 +5915,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5504,7 +5925,7 @@
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -5514,7 +5935,7 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -5524,7 +5945,7 @@
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -5534,7 +5955,7 @@
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -5544,7 +5965,7 @@
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -5554,7 +5975,7 @@
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -5564,7 +5985,7 @@
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -5574,7 +5995,7 @@
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -5584,7 +6005,7 @@
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>

</xml_diff>

<commit_message>
change details about nodejs and improve the file structure
</commit_message>
<xml_diff>
--- a/Git Project Management Tool/git.xlsx
+++ b/Git Project Management Tool/git.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jansson\Desktop\Full-stack\Git Project Management Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F83471-B8E9-408B-BDB1-521839822C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9051D1A0-43F1-4925-85AB-FAE559D39D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="导航栏" sheetId="1" r:id="rId1"/>
@@ -3793,7 +3793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D25297-5FB8-41DB-829B-F573AEFAADB2}">
   <dimension ref="B2:AA73"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
@@ -3993,7 +3993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17947A92-9EE2-41F6-B11F-1071544CFE37}">
   <dimension ref="C2:P127"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O4" sqref="O4:W9"/>
     </sheetView>
   </sheetViews>
@@ -4384,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC8E6EB-D299-468C-92E1-93201DF9EC15}">
   <dimension ref="E2:W109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L106" sqref="L106"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="S80" sqref="S80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>